<commit_message>
Changed S2F from 1m avg to 12m avg
Signed-off-by: NickChubb27 <joe34burnett@gmail.com>
</commit_message>
<xml_diff>
--- a/extra/sf_predictivePower.xlsx
+++ b/extra/sf_predictivePower.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZBook15\Documents\Bitcoin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZBook15\Documents\Bitcoin\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2030A16B-89FD-4EBB-8B60-0BDEF17DEB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2F23A-1659-4347-AEB3-F7382E748EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CBDF1AEE-9511-4F64-9B1E-33F48A0F4FFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{CBDF1AEE-9511-4F64-9B1E-33F48A0F4FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="PreHalving" sheetId="2" r:id="rId1"/>
-    <sheet name="PreHalving - Remove Outliers" sheetId="11" r:id="rId2"/>
-    <sheet name="PreHalving + First Halving" sheetId="4" r:id="rId3"/>
-    <sheet name="First Halving + Second Halving" sheetId="5" r:id="rId4"/>
-    <sheet name="AllData" sheetId="1" r:id="rId5"/>
-    <sheet name="AllData - Remove early" sheetId="10" r:id="rId6"/>
-    <sheet name="Trend" sheetId="9" r:id="rId7"/>
-    <sheet name="PlanB" sheetId="6" r:id="rId8"/>
-    <sheet name="April 2020" sheetId="7" r:id="rId9"/>
-    <sheet name="April 2020 - PlanB" sheetId="8" r:id="rId10"/>
+    <sheet name="PreHalving (SFW)" sheetId="12" r:id="rId2"/>
+    <sheet name="PreHalving - Remove Outliers" sheetId="11" r:id="rId3"/>
+    <sheet name="PreHalving + First Halving" sheetId="4" r:id="rId4"/>
+    <sheet name="First Halving + Second Halving" sheetId="5" r:id="rId5"/>
+    <sheet name="AllData" sheetId="1" r:id="rId6"/>
+    <sheet name="AllData - Remove early" sheetId="10" r:id="rId7"/>
+    <sheet name="Trend" sheetId="9" r:id="rId8"/>
+    <sheet name="PlanB" sheetId="6" r:id="rId9"/>
+    <sheet name="April 2020" sheetId="7" r:id="rId10"/>
+    <sheet name="April 2020 - PlanB" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="18">
   <si>
     <t>intercept</t>
   </si>
@@ -474,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>14.05</v>
+        <v>15.37</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -503,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3.9</v>
+        <v>3.78</v>
       </c>
       <c r="D2">
         <v>2011</v>
@@ -517,18 +518,18 @@
       </c>
       <c r="G2">
         <f>F2*$B$2+$B$1</f>
-        <v>17.623533854309205</v>
+        <v>18.833578966484303</v>
       </c>
       <c r="H2" s="2">
         <f>EXP(G2)</f>
-        <v>45061277.980140433</v>
+        <v>151119121.28913698</v>
       </c>
       <c r="I2" s="3">
         <v>7300000</v>
       </c>
       <c r="J2" s="1">
         <f>H2/I2</f>
-        <v>6.172777805498689</v>
+        <v>20.701249491662601</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -544,22 +545,22 @@
       </c>
       <c r="G3">
         <f>F3*$B$2+$B$1</f>
-        <v>22.350103652812145</v>
+        <v>23.414715848110234</v>
       </c>
       <c r="H3" s="2">
         <f>EXP(G3)</f>
-        <v>5087760817.8664589</v>
+        <v>14753052509.389925</v>
       </c>
       <c r="I3" s="3">
         <v>11000000</v>
       </c>
       <c r="J3" s="1">
         <f>H3/I3</f>
-        <v>462.52371071513261</v>
+        <v>1341.1865917627204</v>
       </c>
       <c r="K3">
         <f>J3/J2</f>
-        <v>74.929590095259556</v>
+        <v>64.787712080030786</v>
       </c>
       <c r="L3" t="s">
         <v>17</v>
@@ -584,22 +585,22 @@
       </c>
       <c r="G4">
         <f>F4*$B$2+$B$1</f>
-        <v>26.603615716985985</v>
+        <v>27.537350618001796</v>
       </c>
       <c r="H4" s="2">
         <f>EXP(G4)</f>
-        <v>357934453923.85156</v>
+        <v>910582751719.02991</v>
       </c>
       <c r="I4" s="3">
         <v>16000000</v>
       </c>
       <c r="J4" s="1">
         <f>H4/I4</f>
-        <v>22370.903370240721</v>
+        <v>56911.421982439366</v>
       </c>
       <c r="K4">
         <f>J4/J3</f>
-        <v>48.367041195902956</v>
+        <v>42.433634761916856</v>
       </c>
       <c r="L4" t="s">
         <v>17</v>
@@ -618,22 +619,22 @@
       </c>
       <c r="G5">
         <f>F5*$B$2+$B$1</f>
-        <v>29.306889721169767</v>
+        <v>30.157446960518392</v>
       </c>
       <c r="H5" s="2">
         <f>EXP(G5)</f>
-        <v>5343434469098.6143</v>
+        <v>12508718042277.477</v>
       </c>
       <c r="I5" s="3">
         <v>18320000</v>
       </c>
       <c r="J5" s="1">
         <f>H5/I5</f>
-        <v>291672.18717787194</v>
+        <v>682790.28615051729</v>
       </c>
       <c r="K5">
         <f>J5/J4</f>
-        <v>13.038015602261011</v>
+        <v>11.997420945855115</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -652,22 +653,22 @@
       </c>
       <c r="G6">
         <f>F6*$B$2+$B$1</f>
-        <v>32.010163725353557</v>
+        <v>32.777543303034989</v>
       </c>
       <c r="H6" s="2">
         <f>EXP(G6)</f>
-        <v>79769610364543.797</v>
+        <v>171832847443916.84</v>
       </c>
       <c r="I6" s="3">
         <v>19000000</v>
       </c>
       <c r="J6" s="1">
         <f>H6/I6</f>
-        <v>4198400.545502305</v>
+        <v>9043834.0759956241</v>
       </c>
       <c r="K6">
         <f>J6/J5</f>
-        <v>14.394243709435253</v>
+        <v>13.245405301507118</v>
       </c>
       <c r="L6" t="s">
         <v>17</v>
@@ -686,18 +687,18 @@
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G8" si="1">F7*$B$2+$B$1</f>
-        <v>34.713437729537347</v>
+        <v>35.397639645551578</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ref="H7:H8" si="2">EXP(G7)</f>
-        <v>1190842851074496.8</v>
+        <v>2360475898560446</v>
       </c>
       <c r="I7" s="3">
         <v>19300000</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" ref="J7:J8" si="3">H7/I7</f>
-        <v>61701702.128212266</v>
+        <v>122304450.70261379</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -713,18 +714,18 @@
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>37.416711733721129</v>
+        <v>38.017735988068168</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>1.7777530684612062E+16</v>
+        <v>3.2425968320773452E+16</v>
       </c>
       <c r="I8" s="3">
         <v>19500000</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>911668240.236516</v>
+        <v>1662870170.2960744</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -738,6 +739,172 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565D7DE5-B583-49FC-AC84-35AEDF740846}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>-1.84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3.36</v>
+      </c>
+      <c r="D2">
+        <v>2011</v>
+      </c>
+      <c r="E2">
+        <v>2.5</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="1">
+        <f>EXP($B$1)*E2^($B$2)</f>
+        <v>3.451251293649308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3">
+        <v>8.4</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J8" si="0">EXP($B$1)*E3^($B$2)</f>
+        <v>202.52402705947495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.95</v>
+      </c>
+      <c r="D4">
+        <v>2016</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>7906.3599501941253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>2020</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>81177.816924266299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>2024</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>833485.70038579102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>2028</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>8557737.064987801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>2032</v>
+      </c>
+      <c r="E8">
+        <v>400</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>87865770.989914492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C1CE94-5BF6-442E-860B-988342D66EBB}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -904,10 +1071,295 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9416DC40-2D84-402E-A038-91EBADC777B9}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>15.38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3.79</v>
+      </c>
+      <c r="D2">
+        <v>2011</v>
+      </c>
+      <c r="E2">
+        <v>2.5</v>
+      </c>
+      <c r="F2">
+        <f>LN(E2)</f>
+        <v>0.91629073187415511</v>
+      </c>
+      <c r="G2">
+        <f>F2*$B$2+$B$1</f>
+        <v>18.852741873803048</v>
+      </c>
+      <c r="H2" s="2">
+        <f>EXP(G2)</f>
+        <v>154042927.84947833</v>
+      </c>
+      <c r="I2" s="3">
+        <v>7300000</v>
+      </c>
+      <c r="J2" s="1">
+        <f>H2/I2</f>
+        <v>21.101770938284702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3">
+        <v>8.4</v>
+      </c>
+      <c r="F3">
+        <f>LN(E3)</f>
+        <v>2.1282317058492679</v>
+      </c>
+      <c r="G3">
+        <f>F3*$B$2+$B$1</f>
+        <v>23.445998165168724</v>
+      </c>
+      <c r="H3" s="2">
+        <f>EXP(G3)</f>
+        <v>15221856584.732023</v>
+      </c>
+      <c r="I3" s="3">
+        <v>11000000</v>
+      </c>
+      <c r="J3" s="1">
+        <f>H3/I3</f>
+        <v>1383.8051440665477</v>
+      </c>
+      <c r="K3">
+        <f>J3/J2</f>
+        <v>65.577678201213232</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.92</v>
+      </c>
+      <c r="D4">
+        <v>2016</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <f>LN(E4)</f>
+        <v>3.2188758248682006</v>
+      </c>
+      <c r="G4">
+        <f>F4*$B$2+$B$1</f>
+        <v>27.57953937625048</v>
+      </c>
+      <c r="H4" s="2">
+        <f>EXP(G4)</f>
+        <v>949820993840.97192</v>
+      </c>
+      <c r="I4" s="3">
+        <v>16000000</v>
+      </c>
+      <c r="J4" s="1">
+        <f>H4/I4</f>
+        <v>59363.812115060748</v>
+      </c>
+      <c r="K4">
+        <f>J4/J3</f>
+        <v>42.898967654224819</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>2020</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <f>LN(E5)</f>
+        <v>3.912023005428146</v>
+      </c>
+      <c r="G5">
+        <f>F5*$B$2+$B$1</f>
+        <v>30.206567190572674</v>
+      </c>
+      <c r="H5" s="2">
+        <f>EXP(G5)</f>
+        <v>13138489796053.752</v>
+      </c>
+      <c r="I5" s="3">
+        <v>18320000</v>
+      </c>
+      <c r="J5" s="1">
+        <f>H5/I5</f>
+        <v>717166.47358372004</v>
+      </c>
+      <c r="K5">
+        <f>J5/J4</f>
+        <v>12.080869607795506</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>2024</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <f>LN(E6)</f>
+        <v>4.6051701859880918</v>
+      </c>
+      <c r="G6">
+        <f>F6*$B$2+$B$1</f>
+        <v>32.833595004894867</v>
+      </c>
+      <c r="H6" s="2">
+        <f>EXP(G6)</f>
+        <v>181739417469551.38</v>
+      </c>
+      <c r="I6" s="3">
+        <v>19000000</v>
+      </c>
+      <c r="J6" s="1">
+        <f>H6/I6</f>
+        <v>9565232.4983974416</v>
+      </c>
+      <c r="K6">
+        <f>J6/J5</f>
+        <v>13.33753438110325</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>2028</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F8" si="0">LN(E7)</f>
+        <v>5.2983173665480363</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G8" si="1">F7*$B$2+$B$1</f>
+        <v>35.460622819217058</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H8" si="2">EXP(G7)</f>
+        <v>2513927884778076.5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>19300000</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" ref="J7:J8" si="3">H7/I7</f>
+        <v>130255330.81751692</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>2032</v>
+      </c>
+      <c r="E8">
+        <v>400</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>5.9914645471079817</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>38.087650633539255</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="2"/>
+        <v>3.477414805141898E+16</v>
+      </c>
+      <c r="I8" s="3">
+        <v>19500000</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
+        <v>1783289643.6625118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A797907-874B-406E-A465-C9F1FCE5B69A}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1188,7 +1640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BAA0DF-8FBA-4DC7-A529-D3360B3C6613}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -1457,7 +1909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEEB010-4BE3-4A47-92CF-CFA07E491DE5}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -1714,12 +2166,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA50202-FA56-4480-8EEA-05807CAE84C6}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,7 +2446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54CF96A-D66A-4727-9FF2-1678B586052F}">
   <dimension ref="A1:L9"/>
   <sheetViews>
@@ -2274,7 +2726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146D919C-5E5E-4E4C-83B2-3394E82DAF02}">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -2606,7 +3058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB5A829-DCAC-4B59-B2AC-7D22203C40B8}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -2861,170 +3313,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565D7DE5-B583-49FC-AC84-35AEDF740846}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>-1.84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3.36</v>
-      </c>
-      <c r="D2">
-        <v>2011</v>
-      </c>
-      <c r="E2">
-        <v>2.5</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="1">
-        <f>EXP($B$1)*E2^($B$2)</f>
-        <v>3.451251293649308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D3">
-        <v>2012</v>
-      </c>
-      <c r="E3">
-        <v>8.4</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J8" si="0">EXP($B$1)*E3^($B$2)</f>
-        <v>202.52402705947495</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>0.95</v>
-      </c>
-      <c r="D4">
-        <v>2016</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="1">
-        <f t="shared" si="0"/>
-        <v>7906.3599501941253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <v>2020</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="1">
-        <f t="shared" si="0"/>
-        <v>81177.816924266299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>2024</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="1">
-        <f t="shared" si="0"/>
-        <v>833485.70038579102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D7">
-        <v>2028</v>
-      </c>
-      <c r="E7">
-        <v>200</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="1">
-        <f t="shared" si="0"/>
-        <v>8557737.064987801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D8">
-        <v>2032</v>
-      </c>
-      <c r="E8">
-        <v>400</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="1">
-        <f t="shared" si="0"/>
-        <v>87865770.989914492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>